<commit_message>
updates to dictionary, moon phases added, new excell extraction generated
</commit_message>
<xml_diff>
--- a/workingNotes/emoji-201907.xlsx
+++ b/workingNotes/emoji-201907.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackbowers/Box Sync/Language_Data/Mixtepec_Mixtec/workingNotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D6594C-9EC7-704C-A7CB-85FE3CB598B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42610470-F45C-3143-9FFC-6E8177433DAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11240" yWindow="460" windowWidth="20420" windowHeight="15420" xr2:uid="{44DC68A4-B6C5-5749-A60E-4CCF037E4DB4}"/>
+    <workbookView xWindow="4180" yWindow="460" windowWidth="24680" windowHeight="15420" xr2:uid="{44DC68A4-B6C5-5749-A60E-4CCF037E4DB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="173">
   <si>
     <t>😀</t>
   </si>
@@ -523,6 +523,27 @@
   </si>
   <si>
     <t>(died) nstí'i</t>
+  </si>
+  <si>
+    <t>menguante gibosa</t>
+  </si>
+  <si>
+    <t>cuarto menguante</t>
+  </si>
+  <si>
+    <t>menguante</t>
+  </si>
+  <si>
+    <t>nueva</t>
+  </si>
+  <si>
+    <t>creciente</t>
+  </si>
+  <si>
+    <t>cuarto creciente</t>
+  </si>
+  <si>
+    <t>menguant gibosa</t>
   </si>
 </sst>
 </file>
@@ -916,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1664F94-D246-9A4A-8D0B-E50E44F2B9BE}">
-  <dimension ref="A1:C158"/>
+  <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="241" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.2"/>
@@ -1328,62 +1349,62 @@
         <v>84</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>96</v>
       </c>
@@ -1391,7 +1412,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>97</v>
       </c>
@@ -1401,24 +1422,33 @@
       <c r="C93" s="6" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B94" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B95" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>100</v>
       </c>
@@ -1428,8 +1458,11 @@
       <c r="C96" s="5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>101</v>
       </c>
@@ -1439,84 +1472,93 @@
       <c r="C97" s="5" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B98" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B99" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>113</v>
       </c>
@@ -1753,5 +1795,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>